<commit_message>
downloading data and starting to model
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xplore_idm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xplore_idm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="22">
   <si>
     <t>polio0</t>
   </si>
@@ -84,6 +85,12 @@
   </si>
   <si>
     <t>Difference</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
+  </si>
+  <si>
+    <t>Regression</t>
   </si>
 </sst>
 </file>
@@ -114,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,15 +129,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J24" sqref="I24:J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +447,7 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -436,6 +460,9 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
@@ -448,8 +475,11 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -478,19 +508,34 @@
         <v>11</v>
       </c>
       <c r="K2">
-        <v>0.54</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="L2">
-        <v>5.3999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="M2">
-        <v>0.39100000000000001</v>
+        <v>0.495</v>
       </c>
       <c r="N2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2">
+        <v>0.32</v>
+      </c>
+      <c r="R2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="S2">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="T2">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -519,19 +564,34 @@
         <v>6</v>
       </c>
       <c r="K3">
-        <v>0.66100000000000003</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="L3">
-        <v>2.5000000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="M3">
-        <v>0.28899999999999998</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="N3">
-        <v>5.5E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="R3">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="S3">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="T3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -560,19 +620,34 @@
         <v>12</v>
       </c>
       <c r="K4">
-        <v>0.66200000000000003</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L4">
-        <v>3.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="M4">
-        <v>0.309</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="N4">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="R4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="S4">
+        <v>0.373</v>
+      </c>
+      <c r="T4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -601,19 +676,34 @@
         <v>13</v>
       </c>
       <c r="K5">
-        <v>0.69</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="L5">
-        <v>3.5000000000000003E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="M5">
-        <v>0.34499999999999997</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="N5">
-        <v>6.9000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="R5">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="S5">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="T5">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -642,19 +732,34 @@
         <v>14</v>
       </c>
       <c r="K6">
-        <v>0.76300000000000001</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="L6">
-        <v>2.4E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M6">
-        <v>0.34399999999999997</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="N6">
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="R6">
+        <v>6.3E-2</v>
+      </c>
+      <c r="S6">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="T6">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -683,19 +788,34 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.72699999999999998</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="L7">
-        <v>2.8000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="M7">
-        <v>0.43099999999999999</v>
+        <v>0.501</v>
       </c>
       <c r="N7">
-        <v>5.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="R7">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="S7">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="T7">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -724,19 +844,34 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <v>0.56399999999999995</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="L8">
-        <v>2.1999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M8">
-        <v>0.13200000000000001</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="N8">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.9E-2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="R8">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="S8">
+        <v>-0.04</v>
+      </c>
+      <c r="T8">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -765,19 +900,34 @@
         <v>4</v>
       </c>
       <c r="K9">
-        <v>0.60699999999999998</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="L9">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="M9">
-        <v>5.0000000000000001E-3</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="N9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.9E-2</v>
+      </c>
+      <c r="P9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>0.191</v>
+      </c>
+      <c r="R9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="S9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="T9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -806,19 +956,34 @@
         <v>5</v>
       </c>
       <c r="K10">
-        <v>0.502</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="L10">
-        <v>2.4E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M10">
-        <v>-1.0999999999999999E-2</v>
+        <v>0.2</v>
       </c>
       <c r="N10">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+      <c r="P10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10">
+        <v>0.105</v>
+      </c>
+      <c r="R10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="S10">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T10">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -847,19 +1012,34 @@
         <v>15</v>
       </c>
       <c r="K11">
-        <v>0.79300000000000004</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="L11">
-        <v>2.5999999999999999E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="M11">
-        <v>0.39400000000000002</v>
+        <v>0.499</v>
       </c>
       <c r="N11">
-        <v>7.2999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="R11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="T11">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -888,214 +1068,720 @@
         <v>16</v>
       </c>
       <c r="K12">
-        <v>0.44500000000000001</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="L12">
-        <v>3.2000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M12">
-        <v>0.41799999999999998</v>
+        <v>0.121</v>
       </c>
       <c r="N12">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <v>0.128</v>
+      </c>
+      <c r="R12">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="S12">
+        <v>7.8E-2</v>
+      </c>
+      <c r="T12">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <f>VLOOKUP($A15,$A$2:$E$12,5,0)</f>
         <v>0.60199999999999998</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <f>VLOOKUP($A15,$J$2:$N$12,4,0)</f>
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="D15" s="2">
+        <v>0.501</v>
+      </c>
+      <c r="D15" s="3">
         <f>C15-B15</f>
-        <v>-0.17099999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>-0.10099999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
-        <f t="shared" ref="B16:C25" si="0">VLOOKUP($A16,$A$2:$E$12,5,0)</f>
+      <c r="B16" s="2">
+        <f t="shared" ref="B16:B25" si="0">VLOOKUP($A16,$A$2:$E$12,5,0)</f>
         <v>0.20699999999999999</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <f t="shared" ref="C16:C25" si="1">VLOOKUP($A16,$J$2:$N$12,4,0)</f>
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="D16" s="2">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" ref="D16:D25" si="2">C16-B16</f>
-        <v>-7.4999999999999983E-2</v>
+        <v>-0.215</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D17" s="2">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="2"/>
-        <v>-0.185</v>
+        <v>-1.8999999999999989E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <f t="shared" si="1"/>
-        <v>-1.0999999999999999E-2</v>
-      </c>
-      <c r="D18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="3">
         <f t="shared" si="2"/>
-        <v>-2.8000000000000001E-2</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>0.59099999999999997</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <f t="shared" si="1"/>
-        <v>0.309</v>
-      </c>
-      <c r="D19" s="2">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D19" s="3">
         <f t="shared" si="2"/>
-        <v>-0.28199999999999997</v>
+        <v>-0.12499999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>0.59099999999999997</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <f t="shared" si="1"/>
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="D20" s="2">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="D20" s="3">
         <f t="shared" si="2"/>
-        <v>-0.246</v>
+        <v>-0.18799999999999994</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <f t="shared" si="0"/>
         <v>0.55600000000000005</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <f t="shared" si="1"/>
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="D21" s="2">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D21" s="3">
         <f t="shared" si="2"/>
-        <v>-0.21200000000000008</v>
+        <v>-0.16700000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <f t="shared" si="0"/>
         <v>0.63500000000000001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <f t="shared" si="1"/>
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="D22" s="2">
+        <v>0.495</v>
+      </c>
+      <c r="D22" s="3">
         <f t="shared" si="2"/>
-        <v>-0.24399999999999999</v>
+        <v>-0.14000000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <f t="shared" si="0"/>
         <v>0.47499999999999998</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <f t="shared" si="1"/>
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="D23" s="2">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="D23" s="3">
         <f t="shared" si="2"/>
-        <v>-0.186</v>
+        <v>-6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <f t="shared" si="0"/>
         <v>0.126</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <f t="shared" si="1"/>
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="D24" s="2">
+        <v>0.121</v>
+      </c>
+      <c r="D24" s="3">
         <f t="shared" si="2"/>
-        <v>0.29199999999999998</v>
+        <v>-5.0000000000000044E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <f t="shared" si="0"/>
         <v>0.58799999999999997</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <f t="shared" si="1"/>
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="D25" s="2">
+        <v>0.499</v>
+      </c>
+      <c r="D25" s="3">
         <f t="shared" si="2"/>
-        <v>-0.19399999999999995</v>
+        <v>-8.8999999999999968E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D15:D25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.501</v>
+      </c>
+      <c r="D2">
+        <v>0.495</v>
+      </c>
+      <c r="E2">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="F2">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="H2" s="4">
+        <f>AVERAGE(B2:F2)</f>
+        <v>0.49359999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0.371</v>
+      </c>
+      <c r="C3">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H12" si="0">AVERAGE(B3:F3)</f>
+        <v>0.41459999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E4">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.50739999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.52</v>
+      </c>
+      <c r="F6">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45739999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.372</v>
+      </c>
+      <c r="D7">
+        <v>0.501</v>
+      </c>
+      <c r="E7">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0.255</v>
+      </c>
+      <c r="C8">
+        <v>0.193</v>
+      </c>
+      <c r="D8">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.15</v>
+      </c>
+      <c r="F8">
+        <v>0.191</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15619999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.20659999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+      <c r="E10">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11459999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D11">
+        <v>0.499</v>
+      </c>
+      <c r="E11">
+        <v>0.433</v>
+      </c>
+      <c r="F11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45139999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.121</v>
+      </c>
+      <c r="E12">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <f>VLOOKUP($A15,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="C15" s="2">
+        <f>VLOOKUP($A15,$A$2:$H$12,8,0)</f>
+        <v>0.433</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15-B15</f>
+        <v>-0.16899999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <f>VLOOKUP($A16,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" ref="C16:C25" si="1">VLOOKUP($A16,$A$2:$H$12,8,0)</f>
+        <v>0.15619999999999998</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:D25" si="2">C16-B16</f>
+        <v>-5.0800000000000012E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2">
+        <f>VLOOKUP($A17,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.19</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.20659999999999998</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6599999999999976E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <f>VLOOKUP($A18,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
+        <v>9.7599999999999992E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2">
+        <f>VLOOKUP($A19,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.50739999999999996</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="2"/>
+        <v>-8.3600000000000008E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <f>VLOOKUP($A20,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.14599999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <f>VLOOKUP($A21,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45739999999999997</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.8600000000000076E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2">
+        <f>VLOOKUP($A22,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.14140000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2">
+        <f>VLOOKUP($A23,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41459999999999997</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.0400000000000009E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2">
+        <f>VLOOKUP($A24,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.126</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <f>VLOOKUP($A25,Sheet1!$A$2:$E$12,5,0)</f>
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45139999999999991</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.13660000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed model and made saliency maps
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5850" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="nightlight" sheetId="1" r:id="rId1"/>
+    <sheet name="nightlight2" sheetId="2" r:id="rId2"/>
+    <sheet name="net" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="43">
   <si>
     <t>polio0</t>
   </si>
@@ -94,6 +95,66 @@
   </si>
   <si>
     <t>Outcome</t>
+  </si>
+  <si>
+    <t>Extractor</t>
+  </si>
+  <si>
+    <t>vgg11bn_2_4</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>wt decay</t>
+  </si>
+  <si>
+    <t>batches/epoch</t>
+  </si>
+  <si>
+    <t>lr decay</t>
+  </si>
+  <si>
+    <t>0.8 per 50 epochs</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>Training Loss</t>
+  </si>
+  <si>
+    <t>Test Loss</t>
+  </si>
+  <si>
+    <t>Training R2</t>
+  </si>
+  <si>
+    <t>Last year test r2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    predictor = nn.Sequential(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Linear(n_features, 50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Sigmoid(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Linear(50, 20),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Linear(20, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Linear(n_features, 10),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nn.Linear(10, 1),</t>
   </si>
 </sst>
 </file>
@@ -132,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -155,12 +216,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -169,6 +320,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,7 +3014,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="2">
-        <f>VLOOKUP($A15,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A15,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.60199999999999998</v>
       </c>
       <c r="C15" s="2">
@@ -3154,7 +3317,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="2">
-        <f>VLOOKUP($A16,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A16,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.20699999999999999</v>
       </c>
       <c r="C16" s="2">
@@ -3171,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <f>VLOOKUP($A17,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A17,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.19</v>
       </c>
       <c r="C17" s="2">
@@ -3188,7 +3351,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2">
-        <f>VLOOKUP($A18,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A18,nightlight!$A$2:$E$12,5,0)</f>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="C18" s="2">
@@ -3205,7 +3368,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="2">
-        <f>VLOOKUP($A19,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A19,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.59099999999999997</v>
       </c>
       <c r="C19" s="2">
@@ -3222,7 +3385,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="2">
-        <f>VLOOKUP($A20,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A20,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.59099999999999997</v>
       </c>
       <c r="C20" s="2">
@@ -3239,7 +3402,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="2">
-        <f>VLOOKUP($A21,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A21,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.55600000000000005</v>
       </c>
       <c r="C21" s="2">
@@ -3256,7 +3419,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="2">
-        <f>VLOOKUP($A22,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A22,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.63500000000000001</v>
       </c>
       <c r="C22" s="2">
@@ -3273,7 +3436,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="2">
-        <f>VLOOKUP($A23,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A23,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.47499999999999998</v>
       </c>
       <c r="C23" s="2">
@@ -3290,7 +3453,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="2">
-        <f>VLOOKUP($A24,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A24,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.126</v>
       </c>
       <c r="C24" s="2">
@@ -3307,7 +3470,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="2">
-        <f>VLOOKUP($A25,Sheet1!$A$2:$E$12,5,0)</f>
+        <f>VLOOKUP($A25,nightlight!$A$2:$E$12,5,0)</f>
         <v>0.58799999999999997</v>
       </c>
       <c r="C25" s="2">
@@ -3334,4 +3497,632 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.49320000000000003</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D2" s="18">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.48070000000000002</v>
+      </c>
+      <c r="F2" s="9">
+        <f>VLOOKUP($A2,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.45519999999999999</v>
+      </c>
+      <c r="J2" s="16">
+        <v>0.49890000000000001</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.58220000000000005</v>
+      </c>
+      <c r="M2" s="9">
+        <f>VLOOKUP($A2,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.62960000000000005</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.62060000000000004</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.41010000000000002</v>
+      </c>
+      <c r="F3" s="9">
+        <f>VLOOKUP($A3,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.58809999999999996</v>
+      </c>
+      <c r="J3" s="16">
+        <v>0.62709999999999999</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.42620000000000002</v>
+      </c>
+      <c r="M3" s="9">
+        <f>VLOOKUP($A3,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.48139999999999999</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.73550000000000004</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.55069999999999997</v>
+      </c>
+      <c r="F4" s="9">
+        <f>VLOOKUP($A4,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.48459999999999998</v>
+      </c>
+      <c r="J4" s="16">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0.72589999999999999</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="M4" s="9">
+        <f>VLOOKUP($A4,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.52949999999999997</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.57279999999999998</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.65590000000000004</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.49059999999999998</v>
+      </c>
+      <c r="F5" s="9">
+        <f>VLOOKUP($A5,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.50960000000000005</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0.56330000000000002</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.7319</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.53380000000000005</v>
+      </c>
+      <c r="M5" s="9">
+        <f>VLOOKUP($A5,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.55330000000000001</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.59079999999999999</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.63549999999999995</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.46750000000000003</v>
+      </c>
+      <c r="F6" s="9">
+        <f>VLOOKUP($A6,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.54979999999999996</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0.59030000000000005</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.64870000000000005</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.46689999999999998</v>
+      </c>
+      <c r="M6" s="9">
+        <f>VLOOKUP($A6,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.58240000000000003</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.5998</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.51290000000000002</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="F7" s="9">
+        <f>VLOOKUP($A7,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.54590000000000005</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0.57879999999999998</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0.67190000000000005</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.49759999999999999</v>
+      </c>
+      <c r="M7" s="9">
+        <f>VLOOKUP($A7,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.50490000000000002</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.53659999999999997</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.37730000000000002</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="F8" s="9">
+        <f>VLOOKUP($A8,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.51259999999999994</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.54330000000000001</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0.31240000000000001</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.1242</v>
+      </c>
+      <c r="M8" s="9">
+        <f>VLOOKUP($A8,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.61309999999999998</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.38219999999999998</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.14069999999999999</v>
+      </c>
+      <c r="F9" s="9">
+        <f>VLOOKUP($A9,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.19</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.61809999999999998</v>
+      </c>
+      <c r="K9" s="18">
+        <v>0.28670000000000001</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="9">
+        <f>VLOOKUP($A9,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.6663</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.68969999999999998</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.27189999999999998</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="F10" s="9">
+        <f>VLOOKUP($A10,nightlight!$A$15:$D$25,2,0)</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.6804</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.69159999999999999</v>
+      </c>
+      <c r="K10" s="18">
+        <v>0.13120000000000001</v>
+      </c>
+      <c r="L10" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="M10" s="9">
+        <f>VLOOKUP($A10,nightlight!$A$15:$D$25,2,0)</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.4824</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.62780000000000002</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.47110000000000002</v>
+      </c>
+      <c r="F11" s="9">
+        <f>VLOOKUP($A11,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="K11" s="18">
+        <v>0.69620000000000004</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0.49580000000000002</v>
+      </c>
+      <c r="M11" s="9">
+        <f>VLOOKUP($A11,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.58799999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.48209999999999997</v>
+      </c>
+      <c r="C12" s="17">
+        <v>0.51329999999999998</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="F12" s="11">
+        <f>VLOOKUP($A12,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.126</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.49149999999999999</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0.51880000000000004</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.1268</v>
+      </c>
+      <c r="M12" s="11">
+        <f>VLOOKUP($A12,nightlight!$A$15:$D$25,2,0)</f>
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>1E-3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>500</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>